<commit_message>
Removed stuff which 'got in' from other repos somehow
</commit_message>
<xml_diff>
--- a/inst/extdata/Fogyasztói_árindex_,_1990._évi_bázison.xlsx
+++ b/inst/extdata/Fogyasztói_árindex_,_1990._évi_bázison.xlsx
@@ -4417,8 +4417,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8197e89490dc663f80df425c475dfb63">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57d494f76f6743b951aebebbdbb44cb6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd1a842694638f83c0368e938b836db">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94cc445afcc642aee4df2ae1f5e01e9e" ns2:_="" ns3:_="">
     <xsd:import namespace="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
     <xsd:import namespace="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
     <xsd:element name="properties">
@@ -4440,6 +4440,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4514,6 +4515,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4640,10 +4646,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a95d4ba5-ac50-4ccb-8f38-68d250b34105" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3073c576-dbcc-4dca-a8e5-ccf7a0688d93">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66F949B0-8576-48DF-9576-629D41A1274B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B1CD7F4-D966-4CA2-A812-F7105127EFED}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D92061-CE74-45FD-BD7F-B4F5EC7270A1}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB2BF33-2CE8-4C77-A1A6-4C8FF95B7CC4}"/>
 </file>
</xml_diff>